<commit_message>
[add] 添加 xlsx 工具
</commit_message>
<xml_diff>
--- a/configure/table/define.xlsx
+++ b/configure/table/define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="12840" activeTab="1"/>
+    <workbookView windowWidth="30240" windowHeight="12840"/>
   </bookViews>
   <sheets>
     <sheet name="路由表" sheetId="10" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="配表规则说明" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">全局表!$A$1:$E$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">全局表!$A$1:$E$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -64,16 +64,7 @@
     <t>string</t>
   </si>
   <si>
-    <t>@ServerType</t>
-  </si>
-  <si>
-    <t>@RouteType</t>
-  </si>
-  <si>
-    <t>[]@Reward</t>
-  </si>
-  <si>
-    <t>map[@PropertyType]@Reward</t>
+    <t>[]Reward</t>
   </si>
   <si>
     <t>唯一ID</t>
@@ -980,7 +971,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1000,31 +991,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1033,21 +1006,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1367,216 +1328,113 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="7.28846153846154" style="15" customWidth="1"/>
+    <col min="1" max="1" width="7.28846153846154" style="9" customWidth="1"/>
     <col min="2" max="3" width="9.76923076923077" customWidth="1"/>
     <col min="4" max="4" width="9.13461538461539" customWidth="1"/>
     <col min="5" max="5" width="10.4134615384615" customWidth="1"/>
     <col min="6" max="6" width="9.85576923076923" customWidth="1"/>
-    <col min="7" max="7" width="18.3461538461538" style="15" customWidth="1"/>
-    <col min="8" max="8" width="16.0192307692308" customWidth="1"/>
+    <col min="7" max="7" width="18.3461538461538" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="23" t="s">
+      <c r="D3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="E3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="F3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="G3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="23" t="s">
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="D4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="17">
-        <v>1</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="F4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="G4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="17"/>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="17"/>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="17"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="17"/>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="17"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="17"/>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="17"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="17"/>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="17"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="17"/>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="17"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="17"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="17"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="17"/>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="17"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="17"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="17"/>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="17"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="17"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="17"/>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="17"/>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="17"/>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="17"/>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="17"/>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="17"/>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="17"/>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="17"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="17"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="17"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="17"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="17"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1587,91 +1445,73 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.4" outlineLevelRow="3" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="48.5576923076923" style="19" customWidth="1"/>
-    <col min="2" max="2" width="45.8269230769231" style="19" customWidth="1"/>
-    <col min="3" max="3" width="41.6538461538462" style="20" customWidth="1"/>
-    <col min="4" max="4" width="35.8942307692308" style="18" customWidth="1"/>
-    <col min="5" max="5" width="9" style="17"/>
+    <col min="1" max="1" width="48.5576923076923" style="6" customWidth="1"/>
+    <col min="2" max="2" width="45.8269230769231" style="6" customWidth="1"/>
+    <col min="3" max="3" width="41.6538461538462" style="12" customWidth="1"/>
+    <col min="4" max="4" width="35.8942307692308" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9" style="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.6" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="2" ht="17.6" spans="1:4">
+      <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="C2" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" ht="17.6" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="9" t="s">
+    </row>
+    <row r="3" ht="17.6" spans="1:4">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="B3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="C3" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" ht="17.6" spans="1:4">
-      <c r="A3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="9" t="s">
+    </row>
+    <row r="4" ht="17.6" spans="1:3">
+      <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="C4" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" ht="17.6" spans="1:3">
-      <c r="A4" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3">
-      <c r="C5" s="21"/>
-    </row>
-    <row r="6" spans="3:3">
-      <c r="C6" s="21"/>
-    </row>
-    <row r="7" spans="3:3">
-      <c r="C7" s="21"/>
-    </row>
-    <row r="8" spans="3:3">
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="3:3">
-      <c r="C9" s="21"/>
-    </row>
-    <row r="10" spans="3:3">
-      <c r="C10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1685,23 +1525,23 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="39.5769230769231" style="17" customWidth="1"/>
+    <col min="1" max="1" width="39.5769230769231" style="9" customWidth="1"/>
     <col min="2" max="2" width="33.0096153846154" customWidth="1"/>
     <col min="3" max="3" width="33.1730769230769" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="18" t="s">
-        <v>40</v>
+      <c r="A1" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="18"/>
+      <c r="A2" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1715,99 +1555,99 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="21.4711538461538" style="15" customWidth="1"/>
-    <col min="2" max="2" width="19.8653846153846" style="15" customWidth="1"/>
-    <col min="3" max="3" width="21.4711538461538" style="15" customWidth="1"/>
-    <col min="4" max="6" width="20.6730769230769" style="15" customWidth="1"/>
-    <col min="7" max="15" width="9.23076923076923" style="15"/>
+    <col min="1" max="1" width="21.4711538461538" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.8653846153846" style="9" customWidth="1"/>
+    <col min="3" max="3" width="21.4711538461538" style="9" customWidth="1"/>
+    <col min="4" max="6" width="20.6730769230769" style="9" customWidth="1"/>
+    <col min="7" max="15" width="9.23076923076923" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="B2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="16" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="16" t="s">
+      <c r="C3" s="10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="16" t="s">
+      <c r="D3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="16" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="15">
-        <v>0</v>
-      </c>
-      <c r="C4" s="15">
-        <v>0</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="15">
-        <v>0</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="15">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="D6" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1823,31 +1663,31 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="37.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="37.0192307692308" style="11" customWidth="1"/>
-    <col min="3" max="3" width="41.8173076923077" style="11" customWidth="1"/>
-    <col min="4" max="4" width="35.7403846153846" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9" style="11"/>
-    <col min="6" max="6" width="9" style="12"/>
+    <col min="1" max="1" width="37.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="37.0192307692308" style="7" customWidth="1"/>
+    <col min="3" max="3" width="41.8173076923077" style="7" customWidth="1"/>
+    <col min="4" max="4" width="35.7403846153846" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9" style="7"/>
+    <col min="6" max="6" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1862,7 +1702,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelCol="5"/>
@@ -1876,202 +1716,202 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="F3" s="9" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="F4" s="8" t="s">
+      <c r="F5" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="6" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="3" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="6" t="s">
+      <c r="B8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="6" t="s">
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6" t="s">
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="7"/>
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="4:4">
-      <c r="D15" s="7"/>
+      <c r="D15" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>